<commit_message>
Committed the updated testcases
</commit_message>
<xml_diff>
--- a/KULS_Sankar/TestData/IjaraJSPaths.xlsx
+++ b/KULS_Sankar/TestData/IjaraJSPaths.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="48" windowWidth="21072" windowHeight="8268" firstSheet="6" activeTab="8"/>
+    <workbookView xWindow="120" yWindow="48" windowWidth="21072" windowHeight="8268" firstSheet="10" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Ijara_loginElements" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,14 @@
     <sheet name="AssetDetails_Elements" sheetId="12" r:id="rId11"/>
     <sheet name="AddressDetails_Elements" sheetId="13" r:id="rId12"/>
     <sheet name="RepaymentMode_Elements" sheetId="14" r:id="rId13"/>
+    <sheet name="ContactDetails_Elements" sheetId="15" r:id="rId14"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1916" uniqueCount="1805">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1966" uniqueCount="1819">
   <si>
     <t>Ijara_LoginFieldName</t>
   </si>
@@ -5441,6 +5442,48 @@
   </si>
   <si>
     <t>customerEmploymentScreen</t>
+  </si>
+  <si>
+    <t>ContactDetails_FieldName</t>
+  </si>
+  <si>
+    <t>consentForPhContact</t>
+  </si>
+  <si>
+    <t>consentForPhContactLabel</t>
+  </si>
+  <si>
+    <t>consentForPhContactDropdown</t>
+  </si>
+  <si>
+    <t>preferedPhContactType</t>
+  </si>
+  <si>
+    <t>preferedPhContactTypeLabel</t>
+  </si>
+  <si>
+    <t>preferedPhContactTypeDropdown</t>
+  </si>
+  <si>
+    <t>preferredtimeofcontact</t>
+  </si>
+  <si>
+    <t>preferredtimeofcontactLabel</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-label[ng-reflect-text="Email Details"]')</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-label[ng-reflect-text="Phone Details"]')</t>
+  </si>
+  <si>
+    <t>phoneDetailsSection</t>
+  </si>
+  <si>
+    <t>emailDetailsSection</t>
+  </si>
+  <si>
+    <t>preferredtimeofcontactInput</t>
   </si>
 </sst>
 </file>
@@ -7576,7 +7619,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -7735,6 +7778,225 @@
       </c>
       <c r="B19" t="s">
         <v>1129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="47.77734375" customWidth="1"/>
+    <col min="2" max="2" width="98" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="3" t="s">
+        <v>1805</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>791</v>
+      </c>
+      <c r="B2" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>792</v>
+      </c>
+      <c r="B3" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>793</v>
+      </c>
+      <c r="B4" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>798</v>
+      </c>
+      <c r="B5" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>799</v>
+      </c>
+      <c r="B6" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>800</v>
+      </c>
+      <c r="B7" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>1806</v>
+      </c>
+      <c r="B8" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>1807</v>
+      </c>
+      <c r="B9" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>1808</v>
+      </c>
+      <c r="B10" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>1809</v>
+      </c>
+      <c r="B11" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>1810</v>
+      </c>
+      <c r="B12" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>1811</v>
+      </c>
+      <c r="B13" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>1812</v>
+      </c>
+      <c r="B14" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>1813</v>
+      </c>
+      <c r="B15" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>1818</v>
+      </c>
+      <c r="B16" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>823</v>
+      </c>
+      <c r="B17" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>824</v>
+      </c>
+      <c r="B18" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>825</v>
+      </c>
+      <c r="B19" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>829</v>
+      </c>
+      <c r="B20" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>830</v>
+      </c>
+      <c r="B21" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>831</v>
+      </c>
+      <c r="B22" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1815</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>1817</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1814</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B25" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -12597,7 +12859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>